<commit_message>
SensAnalysis des Roskoschmodells mit Te, pe und pa als Variablen (Inputs)
</commit_message>
<xml_diff>
--- a/SensAnalysis_example_data.xlsx
+++ b/SensAnalysis_example_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8F20A0-A84F-4090-A888-A31CB12102A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A61B6D-6875-4918-9ADB-96E5D323CD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="3105" windowWidth="21600" windowHeight="11385" tabRatio="642" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="642" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sensData" sheetId="81" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="26">
   <si>
     <t>running costs</t>
   </si>
@@ -95,10 +95,19 @@
     <t>base</t>
   </si>
   <si>
-    <t>a</t>
+    <t>Te</t>
   </si>
   <si>
-    <t>x</t>
+    <t>pe</t>
+  </si>
+  <si>
+    <t>pa</t>
+  </si>
+  <si>
+    <t>group2</t>
+  </si>
+  <si>
+    <t>group3</t>
   </si>
 </sst>
 </file>
@@ -615,7 +624,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -659,21 +668,20 @@
       </c>
       <c r="B2" s="7">
         <f t="shared" ref="B2:B5" si="0">F2*(1-D2)</f>
-        <v>0.7</v>
+        <v>350</v>
       </c>
       <c r="C2" s="7">
         <f>F2*(1+D2)</f>
-        <v>1.3</v>
+        <v>650</v>
       </c>
       <c r="D2" s="5">
-        <f t="shared" ref="D2:D5" si="1">$J$1</f>
         <v>0.3</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="1">
-        <v>1</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -682,34 +690,50 @@
       </c>
       <c r="B3" s="7">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>210</v>
       </c>
       <c r="C3" s="7">
         <f>F3*(1+D3)</f>
-        <v>1.3</v>
+        <v>390</v>
       </c>
       <c r="D3" s="5">
-        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="7">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="C4" s="7">
+        <f>F4*(1+D4)</f>
+        <v>1300</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1000</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="E5" s="3"/>
+      <c r="F5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>

</xml_diff>

<commit_message>
Sens Analyse, inlet pressure, inlet Temperature, pressure ration and mole fractions as input
</commit_message>
<xml_diff>
--- a/SensAnalysis_example_data.xlsx
+++ b/SensAnalysis_example_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D176C1-B313-487F-9593-F611C648137B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF1C925-5A7D-40A1-8C6F-5C3CDC8A0FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="642" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32715" yWindow="3390" windowWidth="21600" windowHeight="11385" tabRatio="642" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sensData" sheetId="81" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="27">
   <si>
     <t>running costs</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>p_ve</t>
+  </si>
+  <si>
+    <t>p_e</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -584,7 +593,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -626,7 +635,7 @@
         <v>278.14999999999998</v>
       </c>
       <c r="C2" s="7">
-        <v>293.14999999999998</v>
+        <v>298.14999999999998</v>
       </c>
       <c r="D2" s="5">
         <v>0.1</v>
@@ -646,7 +655,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="7">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3" s="5">
         <v>0.1</v>
@@ -659,19 +668,40 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="8">
+        <v>200</v>
+      </c>
+      <c r="C4" s="8">
+        <v>300</v>
+      </c>
       <c r="F4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.9</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.4</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="11"/>
     </row>

</xml_diff>

<commit_message>
Try to save the data properly
</commit_message>
<xml_diff>
--- a/SensAnalysis_example_data.xlsx
+++ b/SensAnalysis_example_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87253864-52EA-4C11-8270-55928E56EB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8245D0-5AA0-4693-8FED-99D458C4E6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="642" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="642" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sensData" sheetId="81" r:id="rId1"/>
@@ -23,7 +23,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="26">
   <si>
     <t>running costs</t>
   </si>
@@ -99,9 +98,6 @@
     <t>group2</t>
   </si>
   <si>
-    <t>T_e</t>
-  </si>
-  <si>
     <t>p_ve</t>
   </si>
   <si>
@@ -111,7 +107,7 @@
     <t>a</t>
   </si>
   <si>
-    <t>b</t>
+    <t>dT</t>
   </si>
 </sst>
 </file>
@@ -594,21 +590,21 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.44140625" style="1"/>
+    <col min="2" max="2" width="12.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -628,15 +624,15 @@
       <c r="I1" s="9"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" s="7">
-        <v>278</v>
+        <v>2</v>
       </c>
       <c r="C2" s="7">
-        <v>298</v>
+        <v>25</v>
       </c>
       <c r="D2" s="5">
         <v>0.1</v>
@@ -648,14 +644,14 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="7">
         <v>1.2</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="7">
         <v>8</v>
       </c>
       <c r="D3" s="5">
@@ -668,21 +664,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="8">
+        <v>120</v>
+      </c>
+      <c r="C4" s="8">
+        <v>500</v>
+      </c>
+      <c r="F4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B4" s="8">
-        <v>190</v>
-      </c>
-      <c r="C4" s="8">
-        <v>580</v>
-      </c>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="B5" s="7">
         <v>0.5</v>
@@ -693,107 +689,101 @@
       <c r="E5" s="3"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="7">
-        <v>0.08</v>
-      </c>
-      <c r="C6" s="7">
-        <v>0.4</v>
-      </c>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
       <c r="E6" s="3"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="13"/>
       <c r="C7" s="7"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="E12" s="11"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="E24" s="11"/>
@@ -816,18 +806,18 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.44140625" style="1"/>
+    <col min="2" max="2" width="12.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -851,7 +841,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="e">
         <f t="shared" ref="A2:A8" si="0">F2</f>
         <v>#REF!</v>
@@ -880,7 +870,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -909,7 +899,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -938,7 +928,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -967,7 +957,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -996,7 +986,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1025,7 +1015,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1054,7 +1044,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1080,7 +1070,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1106,7 +1096,7 @@
         <v>398.15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1132,7 +1122,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1158,7 +1148,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1184,7 +1174,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1210,7 +1200,7 @@
         <v>0.99999000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1236,7 +1226,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1262,7 +1252,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1289,7 +1279,7 @@
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1315,82 +1305,82 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="E32" s="11"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="E34" s="11"/>
@@ -1412,18 +1402,18 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.44140625" style="1"/>
+    <col min="2" max="2" width="12.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1447,7 +1437,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="e">
         <f t="shared" ref="A2:A8" si="0">F2</f>
         <v>#REF!</v>
@@ -1475,7 +1465,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1503,7 +1493,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1531,7 +1521,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1559,7 +1549,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1587,7 +1577,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1615,7 +1605,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1643,7 +1633,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1669,7 +1659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1695,7 +1685,7 @@
         <v>398.15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1721,7 +1711,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1747,7 +1737,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1773,7 +1763,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1799,7 +1789,7 @@
         <v>0.98999499999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1825,7 +1815,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1851,7 +1841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1878,7 +1868,7 @@
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1904,82 +1894,82 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="E32" s="11"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="E34" s="11"/>
@@ -2001,18 +1991,18 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.44140625" style="1"/>
+    <col min="2" max="2" width="12.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2036,7 +2026,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="e">
         <f t="shared" ref="A2:A8" si="0">F2</f>
         <v>#REF!</v>
@@ -2064,7 +2054,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -2092,7 +2082,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -2120,7 +2110,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -2148,7 +2138,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -2176,7 +2166,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -2204,7 +2194,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -2232,7 +2222,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -2258,7 +2248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -2284,7 +2274,7 @@
         <v>398.15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -2310,7 +2300,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -2336,7 +2326,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -2362,7 +2352,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -2388,7 +2378,7 @@
         <v>0.99970000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -2414,7 +2404,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -2440,7 +2430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -2467,7 +2457,7 @@
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2493,82 +2483,82 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="E32" s="11"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="E34" s="11"/>

</xml_diff>

<commit_message>
3faches Gemisch, print Befehle entfernt
</commit_message>
<xml_diff>
--- a/SensAnalysis_example_data.xlsx
+++ b/SensAnalysis_example_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7739F70-0D8C-4D7E-80C4-B3BCBDEE9629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78D5DD8-5F18-491E-92A5-5F55E3EA5D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="642" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6420" yWindow="4836" windowWidth="17280" windowHeight="8964" tabRatio="642" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sensData" sheetId="81" r:id="rId1"/>
@@ -23,6 +23,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="26">
   <si>
     <t>running costs</t>
   </si>
@@ -95,19 +96,16 @@
     <t>base</t>
   </si>
   <si>
-    <t>group2</t>
-  </si>
-  <si>
     <t>p_ve</t>
-  </si>
-  <si>
-    <t>dT</t>
   </si>
   <si>
     <t>p_e</t>
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>dT</t>
   </si>
   <si>
     <t>b</t>
@@ -593,21 +591,21 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="12.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -627,9 +625,9 @@
       <c r="I1" s="9"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="7">
         <v>2</v>
@@ -647,29 +645,21 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="7">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" s="7">
-        <v>1.2</v>
-      </c>
-      <c r="C3" s="7">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="B4" s="8">
         <v>150</v>
@@ -679,120 +669,120 @@
       </c>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="7">
         <v>0.5</v>
       </c>
       <c r="C5" s="7">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="7">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="C6" s="7">
-        <v>9.5000000000000001E-2</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="13"/>
       <c r="C7" s="7"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="E12" s="11"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="E24" s="11"/>
@@ -815,18 +805,18 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="12.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -850,7 +840,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="e">
         <f t="shared" ref="A2:A8" si="0">F2</f>
         <v>#REF!</v>
@@ -879,7 +869,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -908,7 +898,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -937,7 +927,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -966,7 +956,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -995,7 +985,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1024,7 +1014,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1053,7 +1043,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1079,7 +1069,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1105,7 +1095,7 @@
         <v>398.15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1131,7 +1121,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1157,7 +1147,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1183,7 +1173,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1209,7 +1199,7 @@
         <v>0.99999000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1235,7 +1225,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1261,7 +1251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1288,7 +1278,7 @@
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1314,82 +1304,82 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="E32" s="11"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="E34" s="11"/>
@@ -1411,18 +1401,18 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="12.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1446,7 +1436,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="e">
         <f t="shared" ref="A2:A8" si="0">F2</f>
         <v>#REF!</v>
@@ -1474,7 +1464,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1502,7 +1492,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1530,7 +1520,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1558,7 +1548,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1586,7 +1576,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1614,7 +1604,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -1642,7 +1632,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1668,7 +1658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1694,7 +1684,7 @@
         <v>398.15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1720,7 +1710,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1746,7 +1736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1772,7 +1762,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1798,7 +1788,7 @@
         <v>0.98999499999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1824,7 +1814,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1850,7 +1840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1877,7 +1867,7 @@
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1903,82 +1893,82 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="E32" s="11"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="E34" s="11"/>
@@ -2000,18 +1990,18 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="12.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2035,7 +2025,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="e">
         <f t="shared" ref="A2:A8" si="0">F2</f>
         <v>#REF!</v>
@@ -2063,7 +2053,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -2091,7 +2081,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -2119,7 +2109,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -2147,7 +2137,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -2175,7 +2165,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -2203,7 +2193,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
@@ -2231,7 +2221,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -2257,7 +2247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -2283,7 +2273,7 @@
         <v>398.15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -2309,7 +2299,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -2335,7 +2325,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -2361,7 +2351,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -2387,7 +2377,7 @@
         <v>0.99970000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -2413,7 +2403,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -2439,7 +2429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -2466,7 +2456,7 @@
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2492,82 +2482,82 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="E32" s="11"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="E34" s="11"/>

</xml_diff>

<commit_message>
Prints entfernt, angepasst damit Daten sauber gespeichert werden
</commit_message>
<xml_diff>
--- a/SensAnalysis_example_data.xlsx
+++ b/SensAnalysis_example_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53622403-B129-42AC-9C55-C7560438E412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A657659A-292B-498F-9CFB-C61AD55319A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="642" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="26">
   <si>
     <t>running costs</t>
   </si>
@@ -102,7 +102,13 @@
     <t>p_e</t>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
     <t>dT</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -585,7 +591,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -621,7 +627,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="7">
         <v>2</v>
@@ -664,16 +670,28 @@
       <c r="F4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.7</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="11"/>
     </row>

</xml_diff>